<commit_message>
Agrego imagenes de cursos
</commit_message>
<xml_diff>
--- a/data/knowledge_base_2025.xlsx
+++ b/data/knowledge_base_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DESCARGAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72FA453-E5AB-42C2-860A-92E8200566A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFA8243-326E-454B-8734-EBAF79400E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34590" yWindow="2580" windowWidth="21600" windowHeight="11295" xr2:uid="{1455C14F-82CE-4757-B50A-A2D08513430A}"/>
+    <workbookView xWindow="6465" yWindow="2325" windowWidth="21600" windowHeight="11295" xr2:uid="{1455C14F-82CE-4757-B50A-A2D08513430A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Objetivo</t>
   </si>
@@ -84,6 +84,18 @@
   </si>
   <si>
     <t>www.powerbi.com</t>
+  </si>
+  <si>
+    <t>Imagen</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/uc?export=download&amp;id=1qRZkP--NUbOelwVH72-V1mZJbDVbWLxQ</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/uc?export=download&amp;id=1RVsSo1fU2Y5I611PdE6wzUP__Yqpu4f4</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/uc?export=download&amp;id=1gVy1A7O5vaJ0VXjSJzHGQTnyEQhUGYds</t>
   </si>
 </sst>
 </file>
@@ -446,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC04321-8D5B-4E19-AD62-3156017BA2BC}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,10 +469,12 @@
     <col min="1" max="1" width="37.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="163.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="43" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -476,8 +490,11 @@
       <c r="E1" t="s">
         <v>12</v>
       </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -493,8 +510,11 @@
       <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -510,8 +530,11 @@
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -526,6 +549,9 @@
       </c>
       <c r="E4" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -535,5 +561,6 @@
     <hyperlink ref="E4" r:id="rId3" xr:uid="{EEA016ED-2995-432D-931C-236A4F868982}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>